<commit_message>
Fixed problem that caused cost function to crash
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>econ_inflation</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>scenario_9</t>
+  </si>
+  <si>
+    <t>econ_program_unitcost_vaccination</t>
   </si>
 </sst>
 </file>
@@ -540,15 +543,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN3"/>
+  <dimension ref="A1:BN4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="BD7" sqref="BD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1095,6 +1098,179 @@
       </c>
       <c r="BE3" s="4">
         <v>116.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>82</v>
+      </c>
+      <c r="F4">
+        <v>82</v>
+      </c>
+      <c r="G4">
+        <v>82</v>
+      </c>
+      <c r="H4">
+        <v>82</v>
+      </c>
+      <c r="I4">
+        <v>82</v>
+      </c>
+      <c r="J4">
+        <v>82</v>
+      </c>
+      <c r="K4">
+        <v>82</v>
+      </c>
+      <c r="L4">
+        <v>82</v>
+      </c>
+      <c r="M4">
+        <v>82</v>
+      </c>
+      <c r="N4">
+        <v>82</v>
+      </c>
+      <c r="O4">
+        <v>82</v>
+      </c>
+      <c r="P4">
+        <v>82</v>
+      </c>
+      <c r="Q4">
+        <v>82</v>
+      </c>
+      <c r="R4">
+        <v>82</v>
+      </c>
+      <c r="S4">
+        <v>82</v>
+      </c>
+      <c r="T4">
+        <v>82</v>
+      </c>
+      <c r="U4">
+        <v>82</v>
+      </c>
+      <c r="V4">
+        <v>82</v>
+      </c>
+      <c r="W4">
+        <v>82</v>
+      </c>
+      <c r="X4">
+        <v>82</v>
+      </c>
+      <c r="Y4">
+        <v>82</v>
+      </c>
+      <c r="Z4">
+        <v>82</v>
+      </c>
+      <c r="AA4">
+        <v>82</v>
+      </c>
+      <c r="AB4">
+        <v>82</v>
+      </c>
+      <c r="AC4">
+        <v>82</v>
+      </c>
+      <c r="AD4">
+        <v>82</v>
+      </c>
+      <c r="AE4">
+        <v>82</v>
+      </c>
+      <c r="AF4">
+        <v>82</v>
+      </c>
+      <c r="AG4">
+        <v>82</v>
+      </c>
+      <c r="AH4">
+        <v>82</v>
+      </c>
+      <c r="AI4">
+        <v>82</v>
+      </c>
+      <c r="AJ4">
+        <v>82</v>
+      </c>
+      <c r="AK4">
+        <v>82</v>
+      </c>
+      <c r="AL4">
+        <v>82</v>
+      </c>
+      <c r="AM4">
+        <v>82</v>
+      </c>
+      <c r="AN4">
+        <v>82</v>
+      </c>
+      <c r="AO4">
+        <v>82</v>
+      </c>
+      <c r="AP4">
+        <v>82</v>
+      </c>
+      <c r="AQ4">
+        <v>82</v>
+      </c>
+      <c r="AR4">
+        <v>82</v>
+      </c>
+      <c r="AS4">
+        <v>82</v>
+      </c>
+      <c r="AT4">
+        <v>82</v>
+      </c>
+      <c r="AU4">
+        <v>82</v>
+      </c>
+      <c r="AV4">
+        <v>82</v>
+      </c>
+      <c r="AW4">
+        <v>82</v>
+      </c>
+      <c r="AX4">
+        <v>82</v>
+      </c>
+      <c r="AY4">
+        <v>82</v>
+      </c>
+      <c r="AZ4">
+        <v>82</v>
+      </c>
+      <c r="BA4">
+        <v>82</v>
+      </c>
+      <c r="BB4">
+        <v>82</v>
+      </c>
+      <c r="BC4">
+        <v>82</v>
+      </c>
+      <c r="BD4">
+        <v>82</v>
+      </c>
+      <c r="BE4">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Both methods of estimating costs are now running fine for BCG
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>econ_inflation</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>econ_program_unitcost_vaccination</t>
+  </si>
+  <si>
+    <t>econ_program_totalcost_vaccination</t>
   </si>
 </sst>
 </file>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN4"/>
+  <dimension ref="A1:BR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BD7" sqref="BD7"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AK5" sqref="AK5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +557,7 @@
     <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -726,35 +729,47 @@
       <c r="BE1" s="10">
         <v>2015</v>
       </c>
-      <c r="BF1" s="10" t="s">
+      <c r="BF1" s="10">
+        <v>2020</v>
+      </c>
+      <c r="BG1" s="10">
+        <v>2025</v>
+      </c>
+      <c r="BH1" s="10">
+        <v>2030</v>
+      </c>
+      <c r="BI1" s="10">
+        <v>2035</v>
+      </c>
+      <c r="BJ1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="BG1" s="10" t="s">
+      <c r="BK1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="BH1" s="10" t="s">
+      <c r="BL1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="BI1" s="10" t="s">
+      <c r="BM1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="BJ1" s="10" t="s">
+      <c r="BN1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="BK1" s="10" t="s">
+      <c r="BO1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="BL1" s="10" t="s">
+      <c r="BP1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="BM1" s="10" t="s">
+      <c r="BQ1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="BN1" s="10" t="s">
+      <c r="BR1" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,8 +941,20 @@
       <c r="BE2" s="6">
         <v>1.4E-2</v>
       </c>
+      <c r="BF2" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="BG2" s="6">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="BH2" s="6">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="BI2" s="6">
+        <v>3.3000000000000002E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1099,8 +1126,20 @@
       <c r="BE3" s="4">
         <v>116.4</v>
       </c>
+      <c r="BF3" s="4">
+        <v>120</v>
+      </c>
+      <c r="BG3" s="4">
+        <v>124</v>
+      </c>
+      <c r="BH3" s="4">
+        <v>128</v>
+      </c>
+      <c r="BI3" s="4">
+        <v>132</v>
+      </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1271,6 +1310,83 @@
       </c>
       <c r="BE4">
         <v>82</v>
+      </c>
+      <c r="BF4">
+        <v>82</v>
+      </c>
+      <c r="BG4">
+        <v>82</v>
+      </c>
+      <c r="BH4">
+        <v>82</v>
+      </c>
+      <c r="BI4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>100000</v>
+      </c>
+      <c r="L5">
+        <v>200000</v>
+      </c>
+      <c r="Q5">
+        <v>200000</v>
+      </c>
+      <c r="V5">
+        <v>350000</v>
+      </c>
+      <c r="AF5">
+        <v>400000</v>
+      </c>
+      <c r="AK5">
+        <v>410000</v>
+      </c>
+      <c r="AP5">
+        <v>430000</v>
+      </c>
+      <c r="AZ5">
+        <v>500000</v>
+      </c>
+      <c r="BE5">
+        <v>500000</v>
+      </c>
+      <c r="BF5">
+        <v>430000</v>
+      </c>
+      <c r="BH5">
+        <v>400000</v>
+      </c>
+      <c r="BI5">
+        <v>400000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More realistic cost estimations of BCG with literature-informed unit cost
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -16,6 +16,142 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tan Doan</author>
+  </authors>
+  <commentList>
+    <comment ref="T4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tan Doan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Indonesia 
+Lancet 2006; 367: 1173–80</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AM4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tan Doan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Chzech republic 
+Lancet 2006; 367: 1173–80</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AO4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tan Doan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Salvado
+Lancet Infect Dis 2012;
+12: 300–06</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BA4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tan Doan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Zambia. 
+Expert Rev Vaccines 11(3), 2012 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BB4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tan Doan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+South Africa 
+Ditkowsky JB, Schwartzman K (2014) PLoS ONE 9(1): e83526. doi:10.1371/journal.pone.0083526</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
@@ -77,7 +213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +269,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -545,11 +694,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AK5" sqref="AK5"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="BH10" sqref="BH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,16 +1091,16 @@
         <v>1.4E-2</v>
       </c>
       <c r="BF2" s="6">
-        <v>0.03</v>
+        <v>1.4E-2</v>
       </c>
       <c r="BG2" s="6">
-        <v>3.3000000000000002E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="BH2" s="6">
-        <v>3.3000000000000002E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="BI2" s="6">
-        <v>3.3000000000000002E-2</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="3" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1127,16 +1276,16 @@
         <v>116.4</v>
       </c>
       <c r="BF3" s="4">
-        <v>120</v>
+        <v>116.4</v>
       </c>
       <c r="BG3" s="4">
-        <v>124</v>
+        <v>116.4</v>
       </c>
       <c r="BH3" s="4">
-        <v>128</v>
+        <v>116.4</v>
       </c>
       <c r="BI3" s="4">
-        <v>132</v>
+        <v>116.4</v>
       </c>
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.25">
@@ -1153,175 +1302,46 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>82</v>
-      </c>
-      <c r="J4">
-        <v>82</v>
-      </c>
-      <c r="K4">
-        <v>82</v>
-      </c>
-      <c r="L4">
-        <v>82</v>
-      </c>
-      <c r="M4">
-        <v>82</v>
-      </c>
-      <c r="N4">
-        <v>82</v>
-      </c>
-      <c r="O4">
-        <v>82</v>
-      </c>
-      <c r="P4">
-        <v>82</v>
-      </c>
-      <c r="Q4">
-        <v>82</v>
-      </c>
-      <c r="R4">
-        <v>82</v>
-      </c>
-      <c r="S4">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>82</v>
-      </c>
-      <c r="U4">
-        <v>82</v>
-      </c>
-      <c r="V4">
-        <v>82</v>
-      </c>
-      <c r="W4">
-        <v>82</v>
-      </c>
-      <c r="X4">
-        <v>82</v>
-      </c>
-      <c r="Y4">
-        <v>82</v>
-      </c>
-      <c r="Z4">
-        <v>82</v>
-      </c>
-      <c r="AA4">
-        <v>82</v>
-      </c>
-      <c r="AB4">
-        <v>82</v>
-      </c>
-      <c r="AC4">
-        <v>82</v>
-      </c>
-      <c r="AD4">
-        <v>82</v>
-      </c>
-      <c r="AE4">
-        <v>82</v>
-      </c>
-      <c r="AF4">
-        <v>82</v>
-      </c>
-      <c r="AG4">
-        <v>82</v>
-      </c>
-      <c r="AH4">
-        <v>82</v>
-      </c>
-      <c r="AI4">
-        <v>82</v>
-      </c>
-      <c r="AJ4">
-        <v>82</v>
-      </c>
-      <c r="AK4">
-        <v>82</v>
-      </c>
-      <c r="AL4">
-        <v>82</v>
+        <v>1.8</v>
       </c>
       <c r="AM4">
-        <v>82</v>
-      </c>
-      <c r="AN4">
-        <v>82</v>
+        <v>1.75</v>
       </c>
       <c r="AO4">
-        <v>82</v>
-      </c>
-      <c r="AP4">
-        <v>82</v>
-      </c>
-      <c r="AQ4">
-        <v>82</v>
-      </c>
-      <c r="AR4">
-        <v>82</v>
-      </c>
-      <c r="AS4">
-        <v>82</v>
-      </c>
-      <c r="AT4">
-        <v>82</v>
-      </c>
-      <c r="AU4">
-        <v>82</v>
-      </c>
-      <c r="AV4">
-        <v>82</v>
-      </c>
-      <c r="AW4">
-        <v>82</v>
-      </c>
-      <c r="AX4">
-        <v>82</v>
-      </c>
-      <c r="AY4">
-        <v>82</v>
-      </c>
-      <c r="AZ4">
-        <v>82</v>
-      </c>
-      <c r="BA4">
-        <v>82</v>
+        <v>1.4</v>
       </c>
       <c r="BB4">
-        <v>82</v>
-      </c>
-      <c r="BC4">
-        <v>82</v>
-      </c>
-      <c r="BD4">
-        <v>82</v>
+        <v>2.13</v>
       </c>
       <c r="BE4">
-        <v>82</v>
+        <v>2.5</v>
       </c>
       <c r="BF4">
-        <v>82</v>
+        <v>2.5</v>
       </c>
       <c r="BG4">
-        <v>82</v>
+        <v>2.5</v>
       </c>
       <c r="BH4">
-        <v>82</v>
+        <v>2.5</v>
       </c>
       <c r="BI4">
-        <v>82</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:70" x14ac:dyDescent="0.25">
@@ -1402,6 +1422,7 @@
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Started working on GeneXert cost
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>econ_inflation</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>econ_program_totalcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_program_totalcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_program_unitcost_xpert</t>
   </si>
 </sst>
 </file>
@@ -701,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR7"/>
+  <dimension ref="A1:BR9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,6 +1660,34 @@
       </c>
       <c r="BI7">
         <v>250000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dummy values of Xpert cost for the model to work
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -710,7 +710,7 @@
   <dimension ref="A1:BR9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1674,11 +1674,170 @@
       </c>
       <c r="D8" t="s">
         <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>20.77</v>
+      </c>
+      <c r="BB8">
+        <v>22</v>
+      </c>
+      <c r="BE8">
+        <v>21</v>
+      </c>
+      <c r="BF8">
+        <v>21</v>
+      </c>
+      <c r="BG8">
+        <v>21</v>
+      </c>
+      <c r="BH8">
+        <v>21</v>
+      </c>
+      <c r="BI8">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1688,6 +1847,57 @@
       </c>
       <c r="D9" t="s">
         <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>10000</v>
+      </c>
+      <c r="L9">
+        <v>10000</v>
+      </c>
+      <c r="Q9">
+        <v>30000</v>
+      </c>
+      <c r="V9">
+        <v>50000</v>
+      </c>
+      <c r="AF9">
+        <v>80000</v>
+      </c>
+      <c r="AK9">
+        <v>100000</v>
+      </c>
+      <c r="AP9">
+        <v>100000</v>
+      </c>
+      <c r="AZ9">
+        <v>100000</v>
+      </c>
+      <c r="BE9">
+        <v>110000</v>
+      </c>
+      <c r="BF9">
+        <v>250000</v>
+      </c>
+      <c r="BH9">
+        <v>250000</v>
+      </c>
+      <c r="BI9">
+        <v>250000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished BCG, GXpert, IPT and treatment support
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>econ_inflation</t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t>econ_program_unitcost_xpert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">econ_program_prop_vaccination </t>
+  </si>
+  <si>
+    <t>econ_program_prop_ipt</t>
+  </si>
+  <si>
+    <t>econ_program_prop_xpert</t>
+  </si>
+  <si>
+    <t>econ_program_prop_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_program_unitcost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_program_totalcost_treatment_support</t>
   </si>
 </sst>
 </file>
@@ -707,18 +725,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BR9"/>
+  <dimension ref="A1:BV15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -891,46 +909,58 @@
         <v>2015</v>
       </c>
       <c r="BF1" s="10">
+        <v>2016</v>
+      </c>
+      <c r="BG1" s="10">
+        <v>2017</v>
+      </c>
+      <c r="BH1" s="10">
+        <v>2018</v>
+      </c>
+      <c r="BI1" s="10">
+        <v>2019</v>
+      </c>
+      <c r="BJ1" s="10">
         <v>2020</v>
       </c>
-      <c r="BG1" s="10">
+      <c r="BK1" s="10">
         <v>2025</v>
       </c>
-      <c r="BH1" s="10">
+      <c r="BL1" s="10">
         <v>2030</v>
       </c>
-      <c r="BI1" s="10">
+      <c r="BM1" s="10">
         <v>2035</v>
       </c>
-      <c r="BJ1" s="10" t="s">
+      <c r="BN1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="BK1" s="10" t="s">
+      <c r="BO1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="BL1" s="10" t="s">
+      <c r="BP1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="BM1" s="10" t="s">
+      <c r="BQ1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="BN1" s="10" t="s">
+      <c r="BR1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="BO1" s="10" t="s">
+      <c r="BS1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="BP1" s="10" t="s">
+      <c r="BT1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="BQ1" s="10" t="s">
+      <c r="BU1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="BR1" s="10" t="s">
+      <c r="BV1" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1102,20 +1132,24 @@
       <c r="BE2" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="BF2" s="6">
+      <c r="BF2" s="6"/>
+      <c r="BG2" s="6"/>
+      <c r="BH2" s="6"/>
+      <c r="BI2" s="6"/>
+      <c r="BJ2" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="BG2" s="6">
+      <c r="BK2" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="BH2" s="6">
+      <c r="BL2" s="6">
         <v>1.4E-2</v>
       </c>
-      <c r="BI2" s="6">
+      <c r="BM2" s="6">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:70" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1287,20 +1321,20 @@
       <c r="BE3" s="4">
         <v>116.4</v>
       </c>
-      <c r="BF3" s="4">
+      <c r="BJ3" s="4">
         <v>116.4</v>
       </c>
-      <c r="BG3" s="4">
+      <c r="BK3" s="4">
         <v>116.4</v>
       </c>
-      <c r="BH3" s="4">
+      <c r="BL3" s="4">
         <v>116.4</v>
       </c>
-      <c r="BI3" s="4">
+      <c r="BM3" s="4">
         <v>116.4</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1313,24 +1347,6 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="T4">
         <v>1.8</v>
       </c>
@@ -1346,20 +1362,20 @@
       <c r="BE4">
         <v>2</v>
       </c>
-      <c r="BF4">
-        <v>1</v>
-      </c>
-      <c r="BG4">
-        <v>1</v>
-      </c>
-      <c r="BH4">
-        <v>1</v>
-      </c>
-      <c r="BI4">
+      <c r="BJ4">
+        <v>1</v>
+      </c>
+      <c r="BK4">
+        <v>1</v>
+      </c>
+      <c r="BL4">
+        <v>1</v>
+      </c>
+      <c r="BM4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1372,21 +1388,6 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
       <c r="J5">
         <v>10000</v>
       </c>
@@ -1414,17 +1415,17 @@
       <c r="BE5">
         <v>110000</v>
       </c>
-      <c r="BF5">
+      <c r="BJ5">
         <v>250000</v>
       </c>
-      <c r="BH5">
+      <c r="BL5">
         <v>250000</v>
       </c>
-      <c r="BI5">
+      <c r="BM5">
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1437,144 +1438,6 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>0</v>
-      </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <v>0</v>
-      </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <v>0</v>
-      </c>
-      <c r="AN6">
-        <v>0</v>
-      </c>
-      <c r="AO6">
-        <v>0</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6">
-        <v>0</v>
-      </c>
-      <c r="AS6">
-        <v>0</v>
-      </c>
-      <c r="AT6">
-        <v>0</v>
-      </c>
-      <c r="AU6">
-        <v>0</v>
-      </c>
-      <c r="AV6">
-        <v>0</v>
-      </c>
-      <c r="AW6">
-        <v>0</v>
-      </c>
-      <c r="AX6">
-        <v>0</v>
-      </c>
       <c r="AY6">
         <v>20.77</v>
       </c>
@@ -1584,20 +1447,20 @@
       <c r="BE6">
         <v>21</v>
       </c>
-      <c r="BF6">
+      <c r="BJ6">
         <v>21</v>
       </c>
-      <c r="BG6">
+      <c r="BK6">
         <v>21</v>
       </c>
-      <c r="BH6">
+      <c r="BL6">
         <v>21</v>
       </c>
-      <c r="BI6">
+      <c r="BM6">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1610,21 +1473,6 @@
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
       <c r="J7">
         <v>10000</v>
       </c>
@@ -1652,17 +1500,17 @@
       <c r="BE7">
         <v>110000</v>
       </c>
-      <c r="BF7">
+      <c r="BJ7">
         <v>250000</v>
       </c>
-      <c r="BH7">
+      <c r="BL7">
         <v>250000</v>
       </c>
-      <c r="BI7">
+      <c r="BM7">
         <v>250000</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1675,167 +1523,11 @@
       <c r="D8" t="s">
         <v>1</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
-      <c r="AK8">
-        <v>0</v>
-      </c>
-      <c r="AL8">
-        <v>0</v>
-      </c>
-      <c r="AM8">
-        <v>0</v>
-      </c>
-      <c r="AN8">
-        <v>0</v>
-      </c>
-      <c r="AO8">
-        <v>0</v>
-      </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
-      <c r="AQ8">
-        <v>0</v>
-      </c>
-      <c r="AR8">
-        <v>0</v>
-      </c>
-      <c r="AS8">
-        <v>0</v>
-      </c>
-      <c r="AT8">
-        <v>0</v>
-      </c>
-      <c r="AU8">
-        <v>0</v>
-      </c>
-      <c r="AV8">
-        <v>0</v>
-      </c>
-      <c r="AW8">
-        <v>0</v>
-      </c>
-      <c r="AX8">
-        <v>0</v>
-      </c>
-      <c r="AY8">
-        <v>20.77</v>
-      </c>
       <c r="BB8">
-        <v>22</v>
-      </c>
-      <c r="BE8">
-        <v>21</v>
-      </c>
-      <c r="BF8">
-        <v>21</v>
-      </c>
-      <c r="BG8">
-        <v>21</v>
-      </c>
-      <c r="BH8">
-        <v>21</v>
-      </c>
-      <c r="BI8">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1848,21 +1540,6 @@
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
       <c r="J9">
         <v>10000</v>
       </c>
@@ -1890,14 +1567,284 @@
       <c r="BE9">
         <v>110000</v>
       </c>
-      <c r="BF9">
+      <c r="BJ9">
         <v>250000</v>
       </c>
-      <c r="BH9">
+      <c r="BL9">
         <v>250000</v>
       </c>
-      <c r="BI9">
+      <c r="BM9">
         <v>250000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>25</v>
+      </c>
+      <c r="V10">
+        <v>95</v>
+      </c>
+      <c r="W10">
+        <v>98</v>
+      </c>
+      <c r="X10">
+        <v>98</v>
+      </c>
+      <c r="Y10">
+        <v>99</v>
+      </c>
+      <c r="Z10">
+        <v>94</v>
+      </c>
+      <c r="AA10">
+        <v>99</v>
+      </c>
+      <c r="AB10">
+        <v>96</v>
+      </c>
+      <c r="AC10">
+        <v>98</v>
+      </c>
+      <c r="AD10">
+        <v>99</v>
+      </c>
+      <c r="AE10">
+        <v>99</v>
+      </c>
+      <c r="AF10">
+        <v>99</v>
+      </c>
+      <c r="AG10">
+        <v>99</v>
+      </c>
+      <c r="AH10">
+        <v>98</v>
+      </c>
+      <c r="AI10">
+        <v>99</v>
+      </c>
+      <c r="AJ10">
+        <v>99</v>
+      </c>
+      <c r="AK10">
+        <v>99</v>
+      </c>
+      <c r="AL10">
+        <v>99</v>
+      </c>
+      <c r="AM10">
+        <v>95</v>
+      </c>
+      <c r="AN10">
+        <v>95</v>
+      </c>
+      <c r="AO10">
+        <v>96</v>
+      </c>
+      <c r="AP10">
+        <v>96</v>
+      </c>
+      <c r="AQ10">
+        <v>97</v>
+      </c>
+      <c r="AR10">
+        <v>97</v>
+      </c>
+      <c r="AS10">
+        <v>97</v>
+      </c>
+      <c r="AT10">
+        <v>98</v>
+      </c>
+      <c r="AU10">
+        <v>98</v>
+      </c>
+      <c r="AV10">
+        <v>99</v>
+      </c>
+      <c r="AW10">
+        <v>99</v>
+      </c>
+      <c r="AX10">
+        <v>99</v>
+      </c>
+      <c r="AY10">
+        <v>99</v>
+      </c>
+      <c r="AZ10">
+        <v>99</v>
+      </c>
+      <c r="BA10">
+        <v>99</v>
+      </c>
+      <c r="BB10">
+        <v>99</v>
+      </c>
+      <c r="BC10">
+        <v>99</v>
+      </c>
+      <c r="BD10">
+        <v>99</v>
+      </c>
+      <c r="BE10">
+        <v>100</v>
+      </c>
+      <c r="BJ10">
+        <v>100</v>
+      </c>
+      <c r="BK10">
+        <v>100</v>
+      </c>
+      <c r="BL10">
+        <v>100</v>
+      </c>
+      <c r="BM10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BB11">
+        <v>7</v>
+      </c>
+      <c r="BD11">
+        <v>23.6</v>
+      </c>
+      <c r="BE11">
+        <v>34</v>
+      </c>
+      <c r="BF11">
+        <v>44</v>
+      </c>
+      <c r="BG11">
+        <v>54</v>
+      </c>
+      <c r="BH11">
+        <v>64</v>
+      </c>
+      <c r="BI11">
+        <v>74</v>
+      </c>
+      <c r="BJ11">
+        <v>84</v>
+      </c>
+      <c r="BK11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BE12">
+        <v>0</v>
+      </c>
+      <c r="BF12">
+        <v>70</v>
+      </c>
+      <c r="BG12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD15">
+        <v>0</v>
+      </c>
+      <c r="BE15">
+        <v>0</v>
+      </c>
+      <c r="BF15">
+        <v>50</v>
+      </c>
+      <c r="BG15">
+        <v>70</v>
+      </c>
+      <c r="BH15">
+        <v>90</v>
+      </c>
+      <c r="BI15">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Economic analysis using new cost formula as discuss with Romain in Townsville
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="time_variants" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>econ_inflation</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>econ_program_totalcost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_program_reflectioncost_vaccination</t>
+  </si>
+  <si>
+    <t>econ_program_reflectioncost_ipt</t>
+  </si>
+  <si>
+    <t>econ_program_reflectioncost_xpert</t>
+  </si>
+  <si>
+    <t>econ_program_reflectioncost_treatment_support</t>
   </si>
 </sst>
 </file>
@@ -725,15 +737,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BV15"/>
+  <dimension ref="A1:BV19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="BK22" sqref="BK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1347,6 +1359,24 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1.8</v>
+      </c>
       <c r="T4">
         <v>1.8</v>
       </c>
@@ -1388,6 +1418,21 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
       <c r="J5">
         <v>10000</v>
       </c>
@@ -1427,7 +1472,7 @@
     </row>
     <row r="6" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1438,31 +1483,85 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>10000</v>
+      </c>
+      <c r="J6">
+        <v>10000</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
       <c r="AY6">
-        <v>20.77</v>
+        <v>0</v>
       </c>
       <c r="BB6">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="BE6">
-        <v>21</v>
-      </c>
-      <c r="BJ6">
-        <v>21</v>
-      </c>
-      <c r="BK6">
-        <v>21</v>
-      </c>
-      <c r="BL6">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
+      <c r="BI6">
+        <v>0</v>
       </c>
       <c r="BM6">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -1473,46 +1572,31 @@
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="J7">
-        <v>10000</v>
-      </c>
-      <c r="L7">
-        <v>10000</v>
-      </c>
-      <c r="Q7">
-        <v>30000</v>
-      </c>
-      <c r="V7">
-        <v>50000</v>
-      </c>
-      <c r="AF7">
-        <v>80000</v>
-      </c>
-      <c r="AK7">
-        <v>100000</v>
-      </c>
-      <c r="AP7">
-        <v>100000</v>
-      </c>
-      <c r="AZ7">
-        <v>100000</v>
+      <c r="AY7">
+        <v>20.77</v>
+      </c>
+      <c r="BB7">
+        <v>22</v>
       </c>
       <c r="BE7">
-        <v>110000</v>
+        <v>21</v>
       </c>
       <c r="BJ7">
-        <v>250000</v>
+        <v>21</v>
+      </c>
+      <c r="BK7">
+        <v>21</v>
       </c>
       <c r="BL7">
-        <v>250000</v>
+        <v>21</v>
       </c>
       <c r="BM7">
-        <v>250000</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -1523,13 +1607,46 @@
       <c r="D8" t="s">
         <v>1</v>
       </c>
-      <c r="BB8">
-        <v>20</v>
+      <c r="J8">
+        <v>10000</v>
+      </c>
+      <c r="L8">
+        <v>10000</v>
+      </c>
+      <c r="Q8">
+        <v>30000</v>
+      </c>
+      <c r="V8">
+        <v>50000</v>
+      </c>
+      <c r="AF8">
+        <v>80000</v>
+      </c>
+      <c r="AK8">
+        <v>100000</v>
+      </c>
+      <c r="AP8">
+        <v>100000</v>
+      </c>
+      <c r="AZ8">
+        <v>100000</v>
+      </c>
+      <c r="BE8">
+        <v>110000</v>
+      </c>
+      <c r="BJ8">
+        <v>250000</v>
+      </c>
+      <c r="BL8">
+        <v>250000</v>
+      </c>
+      <c r="BM8">
+        <v>250000</v>
       </c>
     </row>
     <row r="9" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1540,46 +1657,61 @@
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
+      </c>
+      <c r="AZ9">
         <v>10000</v>
       </c>
-      <c r="L9">
+      <c r="BA9">
         <v>10000</v>
       </c>
-      <c r="Q9">
-        <v>30000</v>
-      </c>
-      <c r="V9">
-        <v>50000</v>
-      </c>
-      <c r="AF9">
-        <v>80000</v>
-      </c>
-      <c r="AK9">
-        <v>100000</v>
-      </c>
-      <c r="AP9">
-        <v>100000</v>
-      </c>
-      <c r="AZ9">
-        <v>100000</v>
+      <c r="BB9">
+        <v>10000</v>
+      </c>
+      <c r="BC9">
+        <v>10000</v>
+      </c>
+      <c r="BD9">
+        <v>8000</v>
       </c>
       <c r="BE9">
-        <v>110000</v>
+        <v>5000</v>
+      </c>
+      <c r="BF9">
+        <v>0</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
+      </c>
+      <c r="BH9">
+        <v>0</v>
+      </c>
+      <c r="BI9">
+        <v>0</v>
       </c>
       <c r="BJ9">
-        <v>250000</v>
+        <v>0</v>
+      </c>
+      <c r="BK9">
+        <v>0</v>
       </c>
       <c r="BL9">
-        <v>250000</v>
+        <v>0</v>
       </c>
       <c r="BM9">
-        <v>250000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -1590,133 +1722,19 @@
       <c r="D10" t="s">
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>25</v>
-      </c>
-      <c r="V10">
-        <v>95</v>
-      </c>
-      <c r="W10">
-        <v>98</v>
-      </c>
-      <c r="X10">
-        <v>98</v>
-      </c>
-      <c r="Y10">
-        <v>99</v>
-      </c>
-      <c r="Z10">
-        <v>94</v>
-      </c>
-      <c r="AA10">
-        <v>99</v>
-      </c>
-      <c r="AB10">
-        <v>96</v>
-      </c>
-      <c r="AC10">
-        <v>98</v>
-      </c>
-      <c r="AD10">
-        <v>99</v>
-      </c>
-      <c r="AE10">
-        <v>99</v>
-      </c>
-      <c r="AF10">
-        <v>99</v>
-      </c>
-      <c r="AG10">
-        <v>99</v>
-      </c>
-      <c r="AH10">
-        <v>98</v>
-      </c>
-      <c r="AI10">
-        <v>99</v>
-      </c>
-      <c r="AJ10">
-        <v>99</v>
-      </c>
-      <c r="AK10">
-        <v>99</v>
-      </c>
-      <c r="AL10">
-        <v>99</v>
-      </c>
-      <c r="AM10">
-        <v>95</v>
-      </c>
-      <c r="AN10">
-        <v>95</v>
-      </c>
-      <c r="AO10">
-        <v>96</v>
-      </c>
-      <c r="AP10">
-        <v>96</v>
-      </c>
-      <c r="AQ10">
-        <v>97</v>
-      </c>
-      <c r="AR10">
-        <v>97</v>
-      </c>
-      <c r="AS10">
-        <v>97</v>
-      </c>
-      <c r="AT10">
-        <v>98</v>
-      </c>
-      <c r="AU10">
-        <v>98</v>
-      </c>
-      <c r="AV10">
-        <v>99</v>
-      </c>
-      <c r="AW10">
-        <v>99</v>
-      </c>
-      <c r="AX10">
-        <v>99</v>
-      </c>
-      <c r="AY10">
-        <v>99</v>
-      </c>
-      <c r="AZ10">
-        <v>99</v>
-      </c>
-      <c r="BA10">
-        <v>99</v>
-      </c>
       <c r="BB10">
-        <v>99</v>
-      </c>
-      <c r="BC10">
-        <v>99</v>
-      </c>
-      <c r="BD10">
-        <v>99</v>
-      </c>
-      <c r="BE10">
-        <v>100</v>
-      </c>
-      <c r="BJ10">
-        <v>100</v>
-      </c>
-      <c r="BK10">
-        <v>100</v>
-      </c>
-      <c r="BL10">
-        <v>100</v>
+        <v>20</v>
+      </c>
+      <c r="BH10">
+        <v>20</v>
       </c>
       <c r="BM10">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -1727,40 +1745,46 @@
       <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="BA11">
-        <v>0</v>
-      </c>
-      <c r="BB11">
-        <v>7</v>
-      </c>
-      <c r="BD11">
-        <v>23.6</v>
+      <c r="J11">
+        <v>10000</v>
+      </c>
+      <c r="L11">
+        <v>10000</v>
+      </c>
+      <c r="Q11">
+        <v>30000</v>
+      </c>
+      <c r="V11">
+        <v>50000</v>
+      </c>
+      <c r="AF11">
+        <v>80000</v>
+      </c>
+      <c r="AK11">
+        <v>100000</v>
+      </c>
+      <c r="AP11">
+        <v>100000</v>
+      </c>
+      <c r="AZ11">
+        <v>100000</v>
       </c>
       <c r="BE11">
-        <v>34</v>
-      </c>
-      <c r="BF11">
-        <v>44</v>
-      </c>
-      <c r="BG11">
-        <v>54</v>
-      </c>
-      <c r="BH11">
-        <v>64</v>
-      </c>
-      <c r="BI11">
-        <v>74</v>
+        <v>110000</v>
       </c>
       <c r="BJ11">
-        <v>84</v>
-      </c>
-      <c r="BK11">
-        <v>100</v>
+        <v>250000</v>
+      </c>
+      <c r="BL11">
+        <v>250000</v>
+      </c>
+      <c r="BM11">
+        <v>250000</v>
       </c>
     </row>
     <row r="12" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1771,19 +1795,49 @@
       <c r="D12" t="s">
         <v>1</v>
       </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="BB12">
+        <v>0</v>
+      </c>
+      <c r="BC12">
+        <v>0</v>
+      </c>
+      <c r="BD12">
+        <v>15000</v>
+      </c>
       <c r="BE12">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="BF12">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="BG12">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="BH12">
+        <v>0</v>
+      </c>
+      <c r="BI12">
+        <v>0</v>
+      </c>
+      <c r="BJ12">
+        <v>0</v>
+      </c>
+      <c r="BK12">
+        <v>0</v>
+      </c>
+      <c r="BL12">
+        <v>0</v>
+      </c>
+      <c r="BM12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1794,13 +1848,133 @@
       <c r="D13" t="s">
         <v>1</v>
       </c>
+      <c r="J13">
+        <v>25</v>
+      </c>
+      <c r="V13">
+        <v>95</v>
+      </c>
+      <c r="W13">
+        <v>98</v>
+      </c>
+      <c r="X13">
+        <v>98</v>
+      </c>
+      <c r="Y13">
+        <v>99</v>
+      </c>
+      <c r="Z13">
+        <v>94</v>
+      </c>
+      <c r="AA13">
+        <v>99</v>
+      </c>
+      <c r="AB13">
+        <v>96</v>
+      </c>
+      <c r="AC13">
+        <v>98</v>
+      </c>
+      <c r="AD13">
+        <v>99</v>
+      </c>
+      <c r="AE13">
+        <v>99</v>
+      </c>
+      <c r="AF13">
+        <v>99</v>
+      </c>
+      <c r="AG13">
+        <v>99</v>
+      </c>
+      <c r="AH13">
+        <v>98</v>
+      </c>
+      <c r="AI13">
+        <v>99</v>
+      </c>
+      <c r="AJ13">
+        <v>99</v>
+      </c>
+      <c r="AK13">
+        <v>99</v>
+      </c>
+      <c r="AL13">
+        <v>99</v>
+      </c>
+      <c r="AM13">
+        <v>95</v>
+      </c>
+      <c r="AN13">
+        <v>95</v>
+      </c>
+      <c r="AO13">
+        <v>96</v>
+      </c>
+      <c r="AP13">
+        <v>96</v>
+      </c>
+      <c r="AQ13">
+        <v>97</v>
+      </c>
+      <c r="AR13">
+        <v>97</v>
+      </c>
+      <c r="AS13">
+        <v>97</v>
+      </c>
+      <c r="AT13">
+        <v>98</v>
+      </c>
+      <c r="AU13">
+        <v>98</v>
+      </c>
+      <c r="AV13">
+        <v>99</v>
+      </c>
+      <c r="AW13">
+        <v>99</v>
+      </c>
+      <c r="AX13">
+        <v>99</v>
+      </c>
+      <c r="AY13">
+        <v>99</v>
+      </c>
+      <c r="AZ13">
+        <v>99</v>
+      </c>
+      <c r="BA13">
+        <v>99</v>
+      </c>
+      <c r="BB13">
+        <v>99</v>
+      </c>
+      <c r="BC13">
+        <v>99</v>
+      </c>
       <c r="BD13">
-        <v>0</v>
+        <v>99</v>
+      </c>
+      <c r="BE13">
+        <v>100</v>
+      </c>
+      <c r="BJ13">
+        <v>100</v>
+      </c>
+      <c r="BK13">
+        <v>100</v>
+      </c>
+      <c r="BL13">
+        <v>100</v>
+      </c>
+      <c r="BM13">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -1811,39 +1985,194 @@
       <c r="D14" t="s">
         <v>1</v>
       </c>
+      <c r="BA14">
+        <v>0</v>
+      </c>
+      <c r="BB14">
+        <v>7</v>
+      </c>
       <c r="BD14">
-        <v>0</v>
+        <v>23.6</v>
+      </c>
+      <c r="BE14">
+        <v>34</v>
+      </c>
+      <c r="BF14">
+        <v>44</v>
+      </c>
+      <c r="BG14">
+        <v>54</v>
+      </c>
+      <c r="BH14">
+        <v>64</v>
+      </c>
+      <c r="BI14">
+        <v>74</v>
+      </c>
+      <c r="BJ14">
+        <v>84</v>
+      </c>
+      <c r="BK14">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="BE15">
+        <v>0</v>
+      </c>
+      <c r="BF15">
+        <v>70</v>
+      </c>
+      <c r="BG15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD16">
+        <v>1000</v>
+      </c>
+      <c r="BE16">
+        <v>1000</v>
+      </c>
+      <c r="BF16">
+        <v>1000</v>
+      </c>
+      <c r="BG16">
+        <v>1000</v>
+      </c>
+      <c r="BH16">
+        <v>1000</v>
+      </c>
+      <c r="BI16">
+        <v>1000</v>
+      </c>
+      <c r="BJ16">
+        <v>1000</v>
+      </c>
+      <c r="BK16">
+        <v>1000</v>
+      </c>
+      <c r="BL16">
+        <v>1000</v>
+      </c>
+      <c r="BM16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD18">
+        <v>0</v>
+      </c>
+      <c r="BE18">
+        <v>0</v>
+      </c>
+      <c r="BF18">
+        <v>0</v>
+      </c>
+      <c r="BG18">
+        <v>0</v>
+      </c>
+      <c r="BH18">
+        <v>0</v>
+      </c>
+      <c r="BI18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="BD15">
-        <v>0</v>
-      </c>
-      <c r="BE15">
-        <v>0</v>
-      </c>
-      <c r="BF15">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="BD19">
+        <v>0</v>
+      </c>
+      <c r="BE19">
+        <v>0</v>
+      </c>
+      <c r="BF19">
         <v>50</v>
       </c>
-      <c r="BG15">
+      <c r="BG19">
         <v>70</v>
       </c>
-      <c r="BH15">
+      <c r="BH19">
         <v>90</v>
       </c>
-      <c r="BI15">
+      <c r="BI19">
+        <v>100</v>
+      </c>
+      <c r="BJ19">
+        <v>100</v>
+      </c>
+      <c r="BK19">
+        <v>100</v>
+      </c>
+      <c r="BL19">
+        <v>100</v>
+      </c>
+      <c r="BM19">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added cost data for ACF
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
   <si>
     <t>econ_inflation</t>
   </si>
@@ -249,6 +249,30 @@
   </si>
   <si>
     <t>econ_program_reflectioncost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_program_prop_smearacf</t>
+  </si>
+  <si>
+    <t>econ_program_totalcost_smearacf</t>
+  </si>
+  <si>
+    <t>econ_program_reflectioncost_smearacf</t>
+  </si>
+  <si>
+    <t>econ_program_unitcost_smearacf</t>
+  </si>
+  <si>
+    <t>econ_program_prop_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_program_totalcost_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_program_reflectioncost_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_program_unitcost_xpertacf</t>
   </si>
 </sst>
 </file>
@@ -737,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BV19"/>
+  <dimension ref="A1:BV27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="BK22" sqref="BK22"/>
+    <sheetView tabSelected="1" topLeftCell="BB6" workbookViewId="0">
+      <selection activeCell="BB23" sqref="BB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2174,6 +2198,202 @@
       </c>
       <c r="BM19">
         <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="BE20">
+        <v>0</v>
+      </c>
+      <c r="BM20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="BE21">
+        <v>0</v>
+      </c>
+      <c r="BM21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="BD22">
+        <v>0</v>
+      </c>
+      <c r="BM22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="BD23">
+        <v>0</v>
+      </c>
+      <c r="BM23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="BB24">
+        <v>0</v>
+      </c>
+      <c r="BM24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="BB25">
+        <v>0</v>
+      </c>
+      <c r="BM25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="BB26">
+        <v>0</v>
+      </c>
+      <c r="BM26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <v>0</v>
+      </c>
+      <c r="BM27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2189,7 +2409,8 @@
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Fix the bug about economics_fiji spreadsheet
Removed a space after the variable 'econ_program_prop_vaccination'
</commit_message>
<xml_diff>
--- a/autumn/xls/economics_fiji.xlsx
+++ b/autumn/xls/economics_fiji.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7410"/>
+    <workbookView xWindow="240" yWindow="132" windowWidth="20112" windowHeight="7416"/>
   </bookViews>
   <sheets>
     <sheet name="time_variants" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
     <author>Tan Doan</author>
   </authors>
   <commentList>
-    <comment ref="T4" authorId="0">
+    <comment ref="T4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM4" authorId="0">
+    <comment ref="AM4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO4" authorId="0">
+    <comment ref="AO4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BA4" authorId="0">
+    <comment ref="BA4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="BB4" authorId="0">
+    <comment ref="BB4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="40">
   <si>
     <t>econ_inflation</t>
   </si>
@@ -221,9 +226,6 @@
     <t>econ_program_unitcost_xpert</t>
   </si>
   <si>
-    <t xml:space="preserve">econ_program_prop_vaccination </t>
-  </si>
-  <si>
     <t>econ_program_prop_ipt</t>
   </si>
   <si>
@@ -273,6 +275,9 @@
   </si>
   <si>
     <t>econ_program_unitcost_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_program_prop_vaccination</t>
   </si>
 </sst>
 </file>
@@ -453,6 +458,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -517,7 +525,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -552,7 +560,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -763,16 +771,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB6" workbookViewId="0">
-      <selection activeCell="BB23" sqref="BB23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -996,7 +1004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1193,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:74" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1370,7 +1378,7 @@
         <v>116.4</v>
       </c>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1429,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1494,9 +1502,9 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1583,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1618,7 +1626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1668,9 +1676,9 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -1733,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1756,7 +1764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1806,9 +1814,9 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -1859,9 +1867,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -1996,9 +2004,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -2040,9 +2048,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -2063,9 +2071,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -2107,9 +2115,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -2124,9 +2132,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -2156,9 +2164,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -2200,182 +2208,182 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="BE20">
+        <v>0</v>
+      </c>
+      <c r="BM20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="BE20">
-        <v>0</v>
-      </c>
-      <c r="BM20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>0</v>
+      </c>
+      <c r="BE21">
+        <v>0</v>
+      </c>
+      <c r="BM21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="AO21">
-        <v>0</v>
-      </c>
-      <c r="BE21">
-        <v>0</v>
-      </c>
-      <c r="BM21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="BD22">
+        <v>0</v>
+      </c>
+      <c r="BM22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="AH22">
-        <v>0</v>
-      </c>
-      <c r="BD22">
-        <v>0</v>
-      </c>
-      <c r="BM22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="BD23">
+        <v>0</v>
+      </c>
+      <c r="BM23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="AL23">
-        <v>0</v>
-      </c>
-      <c r="BD23">
-        <v>0</v>
-      </c>
-      <c r="BM23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="BB24">
+        <v>0</v>
+      </c>
+      <c r="BM24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>36</v>
       </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="BB24">
-        <v>0</v>
-      </c>
-      <c r="BM24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="BB25">
+        <v>0</v>
+      </c>
+      <c r="BM25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="BB25">
-        <v>0</v>
-      </c>
-      <c r="BM25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="BB26">
+        <v>0</v>
+      </c>
+      <c r="BM26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="BB26">
-        <v>0</v>
-      </c>
-      <c r="BM26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>

</xml_diff>